<commit_message>
added allowing get range with empty area (skip_empty_area), expose CalamineError in __init__
</commit_message>
<xml_diff>
--- a/tests/data/base.xlsx
+++ b/tests/data/base.xlsx
@@ -30,10 +30,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;e&quot;AN&quot;"/>
     <numFmt numFmtId="166" formatCode="d/m/yy"/>
+    <numFmt numFmtId="167" formatCode="&quot;ИСТИНА&quot;;&quot;ИСТИНА&quot;;&quot;ЛОЖЬ&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -101,7 +102,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -115,6 +116,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -135,33 +140,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>1.1</v>
       </c>
-      <c r="D1" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="D2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="E2" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F2" s="3" t="n">
         <v>43831</v>
       </c>
     </row>
@@ -187,7 +198,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>